<commit_message>
add comments concerning axioms with disjunctions in RXNO
</commit_message>
<xml_diff>
--- a/docs/Axiomatisation_Rationale.xlsx
+++ b/docs/Axiomatisation_Rationale.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="48" windowWidth="28512" windowHeight="12852"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="28515" windowHeight="12855"/>
   </bookViews>
   <sheets>
     <sheet name="MOP" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="420">
   <si>
     <t>Class</t>
   </si>
@@ -1388,6 +1388,12 @@
   </si>
   <si>
     <t>not necessary, better use "has_synonym" relation</t>
+  </si>
+  <si>
+    <t>subclasses-union-as-equivalent-pattern</t>
+  </si>
+  <si>
+    <t>If it is only a synonym I support JH proposal, otherwise we need another object property to relate this general molecular process to the respective sysnthesis that make use of it.</t>
   </si>
 </sst>
 </file>
@@ -1509,7 +1515,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1554,6 +1560,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1862,23 +1871,23 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="39" style="1" customWidth="1"/>
-    <col min="3" max="3" width="41.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="42.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.44140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="30.88671875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="39.33203125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="11.5546875" style="1"/>
+    <col min="3" max="3" width="41.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="42.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="39.28515625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="13.15" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1904,7 +1913,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="6" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>23</v>
       </c>
@@ -1935,7 +1944,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>28</v>
       </c>
@@ -1963,7 +1972,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="6" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" s="6" customFormat="1" ht="52.9" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
@@ -1980,7 +1989,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="10" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="10" customFormat="1" ht="79.150000000000006" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>34</v>
       </c>
@@ -2109,7 +2118,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="6" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>66</v>
       </c>
@@ -2123,7 +2132,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="10" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" s="10" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>70</v>
       </c>
@@ -2137,7 +2146,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="6" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>74</v>
       </c>
@@ -2151,7 +2160,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="10" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" s="10" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>78</v>
       </c>
@@ -2165,7 +2174,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="6" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>82</v>
       </c>
@@ -2179,7 +2188,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="10" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" s="10" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>86</v>
       </c>
@@ -2193,7 +2202,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="6" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>90</v>
       </c>
@@ -2207,7 +2216,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="10" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" s="10" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>94</v>
       </c>
@@ -2221,7 +2230,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="6" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>98</v>
       </c>
@@ -2235,7 +2244,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="10" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" s="10" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>102</v>
       </c>
@@ -2249,7 +2258,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="6" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>106</v>
       </c>
@@ -2263,7 +2272,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="10" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" s="10" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>110</v>
       </c>
@@ -2277,7 +2286,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="6" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>114</v>
       </c>
@@ -2291,7 +2300,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:4" s="10" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" s="10" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>118</v>
       </c>
@@ -2305,7 +2314,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="30" spans="1:4" s="6" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>122</v>
       </c>
@@ -2319,7 +2328,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="31" spans="1:4" s="10" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" s="10" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>126</v>
       </c>
@@ -2333,7 +2342,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:4" s="6" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>130</v>
       </c>
@@ -2391,24 +2400,24 @@
   <dimension ref="A1:H72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F68" sqref="F68"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F73" sqref="F73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="39" style="1" customWidth="1"/>
-    <col min="3" max="3" width="41.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="42.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.44140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="30.88671875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="39.33203125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="11.5546875" style="1"/>
+    <col min="3" max="3" width="41.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="42.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="39.28515625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="13.15" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2434,7 +2443,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="6" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>23</v>
       </c>
@@ -2447,11 +2456,11 @@
       <c r="D2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E2" s="16" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="10" customFormat="1" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>134</v>
       </c>
@@ -2479,7 +2488,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="10" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="10" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>142</v>
       </c>
@@ -2491,6 +2500,9 @@
       </c>
       <c r="D5" s="15" t="s">
         <v>144</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>418</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>416</v>
@@ -2510,7 +2522,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="10" customFormat="1" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>150</v>
       </c>
@@ -2524,7 +2536,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" s="6" customFormat="1" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>154</v>
       </c>
@@ -2538,7 +2550,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="10" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" s="10" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>158</v>
       </c>
@@ -2550,6 +2562,9 @@
       </c>
       <c r="D9" s="15" t="s">
         <v>165</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>418</v>
       </c>
       <c r="F9" s="10" t="s">
         <v>416</v>
@@ -2569,7 +2584,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="10" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>166</v>
       </c>
@@ -2582,11 +2597,14 @@
       <c r="D11" s="10" t="s">
         <v>169</v>
       </c>
+      <c r="E11" s="16" t="s">
+        <v>418</v>
+      </c>
       <c r="F11" s="10" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="6" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>28</v>
       </c>
@@ -2600,7 +2618,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="10" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>170</v>
       </c>
@@ -2613,11 +2631,14 @@
       <c r="D13" s="10" t="s">
         <v>173</v>
       </c>
+      <c r="E13" s="16" t="s">
+        <v>418</v>
+      </c>
       <c r="F13" s="10" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" s="6" customFormat="1" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>174</v>
       </c>
@@ -2631,7 +2652,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" s="10" customFormat="1" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>178</v>
       </c>
@@ -2645,7 +2666,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" s="6" customFormat="1" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>182</v>
       </c>
@@ -2659,7 +2680,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" s="10" customFormat="1" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>186</v>
       </c>
@@ -2701,7 +2722,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="6" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" s="6" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>198</v>
       </c>
@@ -2715,7 +2736,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="10" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" s="10" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>203</v>
       </c>
@@ -2729,7 +2750,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="6" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>207</v>
       </c>
@@ -2746,7 +2767,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="10" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>212</v>
       </c>
@@ -2763,7 +2784,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="6" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>217</v>
       </c>
@@ -2777,7 +2798,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="10" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" s="10" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>221</v>
       </c>
@@ -2791,7 +2812,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="6" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>225</v>
       </c>
@@ -2804,11 +2825,14 @@
       <c r="D26" s="9" t="s">
         <v>227</v>
       </c>
+      <c r="E26" s="16" t="s">
+        <v>418</v>
+      </c>
       <c r="F26" s="6" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="10" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" s="10" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>229</v>
       </c>
@@ -2822,7 +2846,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="6" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" s="6" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>233</v>
       </c>
@@ -2835,11 +2859,14 @@
       <c r="D28" s="9" t="s">
         <v>235</v>
       </c>
+      <c r="E28" s="16" t="s">
+        <v>418</v>
+      </c>
       <c r="F28" s="6" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="10" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" s="10" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>237</v>
       </c>
@@ -2852,11 +2879,14 @@
       <c r="D29" s="15" t="s">
         <v>239</v>
       </c>
+      <c r="E29" s="16" t="s">
+        <v>418</v>
+      </c>
       <c r="F29" s="10" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="6" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" s="6" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>241</v>
       </c>
@@ -2870,7 +2900,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="10" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>245</v>
       </c>
@@ -2884,7 +2914,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="6" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>249</v>
       </c>
@@ -2898,7 +2928,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="10" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" s="10" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>253</v>
       </c>
@@ -2912,7 +2942,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="6" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>257</v>
       </c>
@@ -2926,7 +2956,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="10" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" s="10" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>261</v>
       </c>
@@ -2940,7 +2970,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="6" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" s="6" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>265</v>
       </c>
@@ -2953,11 +2983,14 @@
       <c r="D36" s="9" t="s">
         <v>267</v>
       </c>
+      <c r="E36" s="16" t="s">
+        <v>418</v>
+      </c>
       <c r="F36" s="6" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="10" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>269</v>
       </c>
@@ -2971,7 +3004,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="6" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>273</v>
       </c>
@@ -2985,7 +3018,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="10" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
         <v>277</v>
       </c>
@@ -2998,11 +3031,14 @@
       <c r="D39" s="10" t="s">
         <v>279</v>
       </c>
+      <c r="E39" s="6" t="s">
+        <v>419</v>
+      </c>
       <c r="F39" s="10" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>281</v>
       </c>
@@ -3016,7 +3052,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
         <v>285</v>
       </c>
@@ -3030,7 +3066,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="6" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>289</v>
       </c>
@@ -3044,7 +3080,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="10" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" s="10" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
         <v>293</v>
       </c>
@@ -3057,11 +3093,14 @@
       <c r="D43" s="15" t="s">
         <v>295</v>
       </c>
+      <c r="E43" s="6" t="s">
+        <v>419</v>
+      </c>
       <c r="F43" s="10" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="6" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>297</v>
       </c>
@@ -3075,7 +3114,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="45" spans="1:6" s="10" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
         <v>301</v>
       </c>
@@ -3088,11 +3127,14 @@
       <c r="D45" s="15" t="s">
         <v>303</v>
       </c>
+      <c r="E45" s="16" t="s">
+        <v>418</v>
+      </c>
       <c r="F45" s="10" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="46" spans="1:6" s="6" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>305</v>
       </c>
@@ -3105,11 +3147,14 @@
       <c r="D46" s="9" t="s">
         <v>307</v>
       </c>
+      <c r="E46" s="16" t="s">
+        <v>418</v>
+      </c>
       <c r="F46" s="6" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="47" spans="1:6" s="10" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" s="10" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
         <v>309</v>
       </c>
@@ -3122,11 +3167,14 @@
       <c r="D47" s="15" t="s">
         <v>311</v>
       </c>
+      <c r="E47" s="16" t="s">
+        <v>418</v>
+      </c>
       <c r="F47" s="10" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="6" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>313</v>
       </c>
@@ -3140,7 +3188,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="49" spans="1:6" s="10" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" s="10" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
         <v>317</v>
       </c>
@@ -3154,7 +3202,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="6" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>321</v>
       </c>
@@ -3168,7 +3216,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="51" spans="1:6" s="10" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" s="10" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
         <v>325</v>
       </c>
@@ -3181,11 +3229,14 @@
       <c r="D51" s="15" t="s">
         <v>327</v>
       </c>
+      <c r="E51" s="16" t="s">
+        <v>418</v>
+      </c>
       <c r="F51" s="10" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="52" spans="1:6" s="6" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" s="6" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>329</v>
       </c>
@@ -3199,7 +3250,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="53" spans="1:6" s="10" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" s="10" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
         <v>333</v>
       </c>
@@ -3213,7 +3264,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="6" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>337</v>
       </c>
@@ -3227,7 +3278,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="10" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" s="10" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
         <v>341</v>
       </c>
@@ -3241,7 +3292,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="56" spans="1:6" s="6" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>345</v>
       </c>
@@ -3255,7 +3306,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="57" spans="1:6" s="10" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" s="10" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
         <v>349</v>
       </c>
@@ -3272,7 +3323,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="58" spans="1:6" s="6" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" s="6" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>354</v>
       </c>
@@ -3286,7 +3337,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="59" spans="1:6" s="10" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" s="10" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
         <v>358</v>
       </c>
@@ -3300,7 +3351,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="60" spans="1:6" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
         <v>362</v>
       </c>
@@ -3314,7 +3365,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="61" spans="1:6" s="10" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" s="10" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
         <v>366</v>
       </c>
@@ -3328,7 +3379,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="62" spans="1:6" s="6" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
         <v>370</v>
       </c>
@@ -3342,7 +3393,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="63" spans="1:6" s="10" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" s="10" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
         <v>374</v>
       </c>
@@ -3356,7 +3407,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="64" spans="1:6" s="6" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
         <v>378</v>
       </c>
@@ -3370,7 +3421,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="65" spans="1:6" s="10" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" s="10" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
         <v>382</v>
       </c>
@@ -3384,7 +3435,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="66" spans="1:6" s="6" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
         <v>386</v>
       </c>
@@ -3398,7 +3449,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="67" spans="1:6" s="10" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" s="10" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
         <v>390</v>
       </c>
@@ -3411,11 +3462,14 @@
       <c r="D67" s="15" t="s">
         <v>392</v>
       </c>
+      <c r="E67" s="16" t="s">
+        <v>418</v>
+      </c>
       <c r="F67" s="10" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="68" spans="1:6" s="6" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>394</v>
       </c>
@@ -3428,11 +3482,14 @@
       <c r="D68" s="9" t="s">
         <v>396</v>
       </c>
+      <c r="E68" s="16" t="s">
+        <v>418</v>
+      </c>
       <c r="F68" s="6" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="69" spans="1:6" s="10" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
         <v>398</v>
       </c>
@@ -3445,11 +3502,14 @@
       <c r="D69" s="15" t="s">
         <v>400</v>
       </c>
+      <c r="E69" s="16" t="s">
+        <v>418</v>
+      </c>
       <c r="F69" s="10" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="70" spans="1:6" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
         <v>402</v>
       </c>
@@ -3462,11 +3522,14 @@
       <c r="D70" s="9" t="s">
         <v>404</v>
       </c>
+      <c r="E70" s="16" t="s">
+        <v>418</v>
+      </c>
       <c r="F70" s="6" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="71" spans="1:6" s="10" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
         <v>406</v>
       </c>
@@ -3483,7 +3546,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="72" spans="1:6" s="6" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
         <v>410</v>
       </c>

</xml_diff>

<commit_message>
add comments concerning axioms with disjunctions in MOP
</commit_message>
<xml_diff>
--- a/docs/Axiomatisation_Rationale.xlsx
+++ b/docs/Axiomatisation_Rationale.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="420">
   <si>
     <t>Class</t>
   </si>
@@ -1870,8 +1870,8 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1926,8 +1926,8 @@
       <c r="D2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>19</v>
+      <c r="E2" s="16" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="10" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
@@ -1956,6 +1956,9 @@
       </c>
       <c r="D4" s="9" t="s">
         <v>22</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="10" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
@@ -2401,7 +2404,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F73" sqref="F73"/>
+      <selection pane="bottomLeft" activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>

</xml_diff>